<commit_message>
VLookUP function use in fees columns
</commit_message>
<xml_diff>
--- a/Capstone Projects/Vlookup and IF function.xlsx
+++ b/Capstone Projects/Vlookup and IF function.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/296e17132c3d1874/Desktop/Client_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e80182422bf530f5/Documents/DeetsDigital/Data/Training/Excel/Capstone Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{B13289C3-4810-4B30-82F2-3229872B3A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61186184-897C-4A90-A59F-9159B1DE7C97}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{B13289C3-4810-4B30-82F2-3229872B3A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{415B0577-2E2D-4178-B316-784F771C84D3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2427,7 +2427,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L293"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2513,6 +2515,10 @@
       <c r="G6" t="s">
         <v>12</v>
       </c>
+      <c r="H6" s="8">
+        <f>VLOOKUP(G6,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
@@ -2543,6 +2549,10 @@
       <c r="G7" t="s">
         <v>18</v>
       </c>
+      <c r="H7" s="8">
+        <f>VLOOKUP(G7,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I7" t="s">
         <v>13</v>
       </c>
@@ -2573,6 +2583,10 @@
       <c r="G8" t="s">
         <v>22</v>
       </c>
+      <c r="H8" s="8">
+        <f>VLOOKUP(G8,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I8" t="s">
         <v>23</v>
       </c>
@@ -2603,6 +2617,10 @@
       <c r="G9" t="s">
         <v>28</v>
       </c>
+      <c r="H9" s="8">
+        <f>VLOOKUP(G9,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I9" t="s">
         <v>29</v>
       </c>
@@ -2636,6 +2654,10 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
+      <c r="H10" s="8">
+        <f>VLOOKUP(G10,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I10" t="s">
         <v>35</v>
       </c>
@@ -2666,6 +2688,10 @@
       <c r="G11" t="s">
         <v>39</v>
       </c>
+      <c r="H11" s="8">
+        <f>VLOOKUP(G11,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I11" t="s">
         <v>13</v>
       </c>
@@ -2696,6 +2722,10 @@
       <c r="G12" t="s">
         <v>43</v>
       </c>
+      <c r="H12" s="8">
+        <f>VLOOKUP(G12,Fees!$A$2:$B$24,2,0)</f>
+        <v>75</v>
+      </c>
       <c r="I12" t="s">
         <v>44</v>
       </c>
@@ -2729,6 +2759,10 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
+      <c r="H13" s="8">
+        <f>VLOOKUP(G13,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -2759,6 +2793,10 @@
       <c r="G14" t="s">
         <v>649</v>
       </c>
+      <c r="H14" s="8">
+        <f>VLOOKUP(G14,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I14" t="s">
         <v>23</v>
       </c>
@@ -2789,6 +2827,10 @@
       <c r="G15" t="s">
         <v>34</v>
       </c>
+      <c r="H15" s="8">
+        <f>VLOOKUP(G15,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I15" t="s">
         <v>53</v>
       </c>
@@ -2819,6 +2861,10 @@
       <c r="G16" t="s">
         <v>650</v>
       </c>
+      <c r="H16" s="8">
+        <f>VLOOKUP(G16,Fees!$A$2:$B$24,2,0)</f>
+        <v>25</v>
+      </c>
       <c r="I16" t="s">
         <v>13</v>
       </c>
@@ -2849,6 +2895,10 @@
       <c r="G17" t="s">
         <v>644</v>
       </c>
+      <c r="H17" s="8">
+        <f>VLOOKUP(G17,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I17" t="s">
         <v>53</v>
       </c>
@@ -2879,6 +2929,10 @@
       <c r="G18" t="s">
         <v>34</v>
       </c>
+      <c r="H18" s="8">
+        <f>VLOOKUP(G18,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I18" t="s">
         <v>13</v>
       </c>
@@ -2909,6 +2963,10 @@
       <c r="G19" t="s">
         <v>647</v>
       </c>
+      <c r="H19" s="8">
+        <f>VLOOKUP(G19,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I19" t="s">
         <v>23</v>
       </c>
@@ -2939,6 +2997,10 @@
       <c r="G20" t="s">
         <v>68</v>
       </c>
+      <c r="H20" s="8">
+        <f>VLOOKUP(G20,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I20" t="s">
         <v>53</v>
       </c>
@@ -2972,6 +3034,10 @@
       <c r="G21" t="s">
         <v>647</v>
       </c>
+      <c r="H21" s="8">
+        <f>VLOOKUP(G21,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I21" t="s">
         <v>23</v>
       </c>
@@ -3002,6 +3068,10 @@
       <c r="G22" t="s">
         <v>39</v>
       </c>
+      <c r="H22" s="8">
+        <f>VLOOKUP(G22,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I22" t="s">
         <v>53</v>
       </c>
@@ -3032,6 +3102,10 @@
       <c r="G23" t="s">
         <v>34</v>
       </c>
+      <c r="H23" s="8">
+        <f>VLOOKUP(G23,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I23" t="s">
         <v>53</v>
       </c>
@@ -3065,6 +3139,10 @@
       <c r="G24" t="s">
         <v>28</v>
       </c>
+      <c r="H24" s="8">
+        <f>VLOOKUP(G24,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I24" t="s">
         <v>53</v>
       </c>
@@ -3095,6 +3173,10 @@
       <c r="G25" t="s">
         <v>646</v>
       </c>
+      <c r="H25" s="8">
+        <f>VLOOKUP(G25,Fees!$A$2:$B$24,2,0)</f>
+        <v>60</v>
+      </c>
       <c r="I25" t="s">
         <v>53</v>
       </c>
@@ -3128,6 +3210,10 @@
       <c r="G26" t="s">
         <v>12</v>
       </c>
+      <c r="H26" s="8">
+        <f>VLOOKUP(G26,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I26" t="s">
         <v>53</v>
       </c>
@@ -3161,6 +3247,10 @@
       <c r="G27" t="s">
         <v>22</v>
       </c>
+      <c r="H27" s="8">
+        <f>VLOOKUP(G27,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I27" t="s">
         <v>23</v>
       </c>
@@ -3194,6 +3284,10 @@
       <c r="G28" t="s">
         <v>91</v>
       </c>
+      <c r="H28" s="8">
+        <f>VLOOKUP(G28,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I28" t="s">
         <v>53</v>
       </c>
@@ -3224,6 +3318,10 @@
       <c r="G29" t="s">
         <v>95</v>
       </c>
+      <c r="H29" s="8">
+        <f>VLOOKUP(G29,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I29" t="s">
         <v>13</v>
       </c>
@@ -3257,6 +3355,10 @@
       <c r="G30" t="s">
         <v>22</v>
       </c>
+      <c r="H30" s="8">
+        <f>VLOOKUP(G30,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I30" t="s">
         <v>53</v>
       </c>
@@ -3290,6 +3392,10 @@
       <c r="G31" t="s">
         <v>95</v>
       </c>
+      <c r="H31" s="8">
+        <f>VLOOKUP(G31,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I31" t="s">
         <v>13</v>
       </c>
@@ -3323,6 +3429,10 @@
       <c r="G32" t="s">
         <v>68</v>
       </c>
+      <c r="H32" s="8">
+        <f>VLOOKUP(G32,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I32" t="s">
         <v>13</v>
       </c>
@@ -3353,6 +3463,10 @@
       <c r="G33" t="s">
         <v>34</v>
       </c>
+      <c r="H33" s="8">
+        <f>VLOOKUP(G33,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I33" t="s">
         <v>13</v>
       </c>
@@ -3386,6 +3500,10 @@
       <c r="G34" t="s">
         <v>28</v>
       </c>
+      <c r="H34" s="8">
+        <f>VLOOKUP(G34,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I34" t="s">
         <v>109</v>
       </c>
@@ -3419,6 +3537,10 @@
       <c r="G35" t="s">
         <v>22</v>
       </c>
+      <c r="H35" s="8">
+        <f>VLOOKUP(G35,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I35" t="s">
         <v>23</v>
       </c>
@@ -3452,6 +3574,10 @@
       <c r="G36" t="s">
         <v>22</v>
       </c>
+      <c r="H36" s="8">
+        <f>VLOOKUP(G36,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I36" t="s">
         <v>13</v>
       </c>
@@ -3485,6 +3611,10 @@
       <c r="G37" t="s">
         <v>119</v>
       </c>
+      <c r="H37" s="8">
+        <f>VLOOKUP(G37,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I37" t="s">
         <v>13</v>
       </c>
@@ -3518,6 +3648,10 @@
       <c r="G38" t="s">
         <v>647</v>
       </c>
+      <c r="H38" s="8">
+        <f>VLOOKUP(G38,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I38" t="s">
         <v>23</v>
       </c>
@@ -3551,6 +3685,10 @@
       <c r="G39" t="s">
         <v>68</v>
       </c>
+      <c r="H39" s="8">
+        <f>VLOOKUP(G39,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I39" t="s">
         <v>23</v>
       </c>
@@ -3584,6 +3722,10 @@
       <c r="G40" t="s">
         <v>12</v>
       </c>
+      <c r="H40" s="8">
+        <f>VLOOKUP(G40,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I40" t="s">
         <v>53</v>
       </c>
@@ -3617,6 +3759,10 @@
       <c r="G41" t="s">
         <v>22</v>
       </c>
+      <c r="H41" s="8">
+        <f>VLOOKUP(G41,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I41" t="s">
         <v>29</v>
       </c>
@@ -3650,6 +3796,10 @@
       <c r="G42" t="s">
         <v>22</v>
       </c>
+      <c r="H42" s="8">
+        <f>VLOOKUP(G42,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I42" t="s">
         <v>29</v>
       </c>
@@ -3683,6 +3833,10 @@
       <c r="G43" t="s">
         <v>650</v>
       </c>
+      <c r="H43" s="8">
+        <f>VLOOKUP(G43,Fees!$A$2:$B$24,2,0)</f>
+        <v>25</v>
+      </c>
       <c r="I43" t="s">
         <v>23</v>
       </c>
@@ -3716,6 +3870,10 @@
       <c r="G44" t="s">
         <v>22</v>
       </c>
+      <c r="H44" s="8">
+        <f>VLOOKUP(G44,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I44" t="s">
         <v>13</v>
       </c>
@@ -3746,6 +3904,10 @@
       <c r="G45" t="s">
         <v>644</v>
       </c>
+      <c r="H45" s="8">
+        <f>VLOOKUP(G45,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I45" t="s">
         <v>23</v>
       </c>
@@ -3779,6 +3941,10 @@
       <c r="G46" t="s">
         <v>647</v>
       </c>
+      <c r="H46" s="8">
+        <f>VLOOKUP(G46,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I46" t="s">
         <v>13</v>
       </c>
@@ -3812,6 +3978,10 @@
       <c r="G47" t="s">
         <v>34</v>
       </c>
+      <c r="H47" s="8">
+        <f>VLOOKUP(G47,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I47" t="s">
         <v>23</v>
       </c>
@@ -3842,6 +4012,10 @@
       <c r="G48" t="s">
         <v>12</v>
       </c>
+      <c r="H48" s="8">
+        <f>VLOOKUP(G48,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I48" t="s">
         <v>13</v>
       </c>
@@ -3875,6 +4049,10 @@
       <c r="G49" t="s">
         <v>650</v>
       </c>
+      <c r="H49" s="8">
+        <f>VLOOKUP(G49,Fees!$A$2:$B$24,2,0)</f>
+        <v>25</v>
+      </c>
       <c r="I49" t="s">
         <v>53</v>
       </c>
@@ -3908,6 +4086,10 @@
       <c r="G50" t="s">
         <v>34</v>
       </c>
+      <c r="H50" s="8">
+        <f>VLOOKUP(G50,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I50" t="s">
         <v>13</v>
       </c>
@@ -3941,6 +4123,10 @@
       <c r="G51" t="s">
         <v>649</v>
       </c>
+      <c r="H51" s="8">
+        <f>VLOOKUP(G51,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I51" t="s">
         <v>23</v>
       </c>
@@ -3971,6 +4157,10 @@
       <c r="G52" t="s">
         <v>34</v>
       </c>
+      <c r="H52" s="8">
+        <f>VLOOKUP(G52,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I52" t="s">
         <v>23</v>
       </c>
@@ -4001,6 +4191,10 @@
       <c r="G53" t="s">
         <v>68</v>
       </c>
+      <c r="H53" s="8">
+        <f>VLOOKUP(G53,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I53" t="s">
         <v>53</v>
       </c>
@@ -4031,6 +4225,10 @@
       <c r="G54" t="s">
         <v>649</v>
       </c>
+      <c r="H54" s="8">
+        <f>VLOOKUP(G54,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I54" t="s">
         <v>23</v>
       </c>
@@ -4064,6 +4262,10 @@
       <c r="G55" t="s">
         <v>647</v>
       </c>
+      <c r="H55" s="8">
+        <f>VLOOKUP(G55,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I55" t="s">
         <v>13</v>
       </c>
@@ -4097,6 +4299,10 @@
       <c r="G56" t="s">
         <v>22</v>
       </c>
+      <c r="H56" s="8">
+        <f>VLOOKUP(G56,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I56" t="s">
         <v>13</v>
       </c>
@@ -4130,6 +4336,10 @@
       <c r="G57" t="s">
         <v>163</v>
       </c>
+      <c r="H57" s="8">
+        <f>VLOOKUP(G57,Fees!$A$2:$B$24,2,0)</f>
+        <v>42</v>
+      </c>
       <c r="I57" t="s">
         <v>53</v>
       </c>
@@ -4160,6 +4370,10 @@
       <c r="G58" t="s">
         <v>647</v>
       </c>
+      <c r="H58" s="8">
+        <f>VLOOKUP(G58,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I58" t="s">
         <v>53</v>
       </c>
@@ -4193,6 +4407,10 @@
       <c r="G59" t="s">
         <v>169</v>
       </c>
+      <c r="H59" s="8">
+        <f>VLOOKUP(G59,Fees!$A$2:$B$24,2,0)</f>
+        <v>23</v>
+      </c>
       <c r="I59" t="s">
         <v>53</v>
       </c>
@@ -4226,6 +4444,10 @@
       <c r="G60" t="s">
         <v>12</v>
       </c>
+      <c r="H60" s="8">
+        <f>VLOOKUP(G60,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I60" t="s">
         <v>53</v>
       </c>
@@ -4256,6 +4478,10 @@
       <c r="G61" t="s">
         <v>647</v>
       </c>
+      <c r="H61" s="8">
+        <f>VLOOKUP(G61,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I61" t="s">
         <v>23</v>
       </c>
@@ -4286,6 +4512,10 @@
       <c r="G62" t="s">
         <v>645</v>
       </c>
+      <c r="H62" s="8">
+        <f>VLOOKUP(G62,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
+      </c>
       <c r="I62" t="s">
         <v>53</v>
       </c>
@@ -4316,6 +4546,10 @@
       <c r="G63" t="s">
         <v>95</v>
       </c>
+      <c r="H63" s="8">
+        <f>VLOOKUP(G63,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I63" t="s">
         <v>23</v>
       </c>
@@ -4349,6 +4583,10 @@
       <c r="G64" t="s">
         <v>184</v>
       </c>
+      <c r="H64" s="8">
+        <f>VLOOKUP(G64,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I64" t="s">
         <v>23</v>
       </c>
@@ -4382,6 +4620,10 @@
       <c r="G65" t="s">
         <v>188</v>
       </c>
+      <c r="H65" s="8">
+        <f>VLOOKUP(G65,Fees!$A$2:$B$24,2,0)</f>
+        <v>68</v>
+      </c>
       <c r="I65" t="s">
         <v>44</v>
       </c>
@@ -4412,6 +4654,10 @@
       <c r="G66" t="s">
         <v>184</v>
       </c>
+      <c r="H66" s="8">
+        <f>VLOOKUP(G66,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I66" t="s">
         <v>13</v>
       </c>
@@ -4442,6 +4688,10 @@
       <c r="G67" t="s">
         <v>95</v>
       </c>
+      <c r="H67" s="8">
+        <f>VLOOKUP(G67,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I67" t="s">
         <v>29</v>
       </c>
@@ -4472,6 +4722,10 @@
       <c r="G68" t="s">
         <v>12</v>
       </c>
+      <c r="H68" s="8">
+        <f>VLOOKUP(G68,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I68" t="s">
         <v>23</v>
       </c>
@@ -4502,6 +4756,10 @@
       <c r="G69" t="s">
         <v>95</v>
       </c>
+      <c r="H69" s="8">
+        <f>VLOOKUP(G69,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I69" t="s">
         <v>53</v>
       </c>
@@ -4532,6 +4790,10 @@
       <c r="G70" t="s">
         <v>647</v>
       </c>
+      <c r="H70" s="8">
+        <f>VLOOKUP(G70,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I70" t="s">
         <v>23</v>
       </c>
@@ -4562,6 +4824,10 @@
       <c r="G71" t="s">
         <v>18</v>
       </c>
+      <c r="H71" s="8">
+        <f>VLOOKUP(G71,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I71" t="s">
         <v>53</v>
       </c>
@@ -4592,6 +4858,10 @@
       <c r="G72" t="s">
         <v>22</v>
       </c>
+      <c r="H72" s="8">
+        <f>VLOOKUP(G72,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I72" t="s">
         <v>23</v>
       </c>
@@ -4622,6 +4892,10 @@
       <c r="G73" t="s">
         <v>34</v>
       </c>
+      <c r="H73" s="8">
+        <f>VLOOKUP(G73,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I73" t="s">
         <v>53</v>
       </c>
@@ -4655,6 +4929,10 @@
       <c r="G74" t="s">
         <v>649</v>
       </c>
+      <c r="H74" s="8">
+        <f>VLOOKUP(G74,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I74" t="s">
         <v>208</v>
       </c>
@@ -4685,6 +4963,10 @@
       <c r="G75" t="s">
         <v>18</v>
       </c>
+      <c r="H75" s="8">
+        <f>VLOOKUP(G75,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I75" t="s">
         <v>23</v>
       </c>
@@ -4715,6 +4997,10 @@
       <c r="G76" t="s">
         <v>647</v>
       </c>
+      <c r="H76" s="8">
+        <f>VLOOKUP(G76,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I76" t="s">
         <v>13</v>
       </c>
@@ -4748,6 +5034,10 @@
       <c r="G77" t="s">
         <v>95</v>
       </c>
+      <c r="H77" s="8">
+        <f>VLOOKUP(G77,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I77" t="s">
         <v>53</v>
       </c>
@@ -4781,6 +5071,10 @@
       <c r="G78" t="s">
         <v>648</v>
       </c>
+      <c r="H78" s="8">
+        <f>VLOOKUP(G78,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I78" t="s">
         <v>53</v>
       </c>
@@ -4814,6 +5108,10 @@
       <c r="G79" t="s">
         <v>95</v>
       </c>
+      <c r="H79" s="8">
+        <f>VLOOKUP(G79,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I79" t="s">
         <v>23</v>
       </c>
@@ -4844,6 +5142,10 @@
       <c r="G80" t="s">
         <v>649</v>
       </c>
+      <c r="H80" s="8">
+        <f>VLOOKUP(G80,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I80" t="s">
         <v>53</v>
       </c>
@@ -4874,6 +5176,10 @@
       <c r="G81" t="s">
         <v>12</v>
       </c>
+      <c r="H81" s="8">
+        <f>VLOOKUP(G81,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I81" t="s">
         <v>13</v>
       </c>
@@ -4907,6 +5213,10 @@
       <c r="G82" t="s">
         <v>228</v>
       </c>
+      <c r="H82" s="8">
+        <f>VLOOKUP(G82,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I82" t="s">
         <v>53</v>
       </c>
@@ -4940,6 +5250,10 @@
       <c r="G83" t="s">
         <v>39</v>
       </c>
+      <c r="H83" s="8">
+        <f>VLOOKUP(G83,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I83" t="s">
         <v>13</v>
       </c>
@@ -4973,6 +5287,10 @@
       <c r="G84" t="s">
         <v>22</v>
       </c>
+      <c r="H84" s="8">
+        <f>VLOOKUP(G84,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I84" t="s">
         <v>23</v>
       </c>
@@ -5003,6 +5321,10 @@
       <c r="G85" t="s">
         <v>22</v>
       </c>
+      <c r="H85" s="8">
+        <f>VLOOKUP(G85,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I85" t="s">
         <v>13</v>
       </c>
@@ -5036,6 +5358,10 @@
       <c r="G86" t="s">
         <v>28</v>
       </c>
+      <c r="H86" s="8">
+        <f>VLOOKUP(G86,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I86" t="s">
         <v>23</v>
       </c>
@@ -5069,6 +5395,10 @@
       <c r="G87" t="s">
         <v>648</v>
       </c>
+      <c r="H87" s="8">
+        <f>VLOOKUP(G87,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I87" t="s">
         <v>53</v>
       </c>
@@ -5099,6 +5429,10 @@
       <c r="G88" t="s">
         <v>34</v>
       </c>
+      <c r="H88" s="8">
+        <f>VLOOKUP(G88,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I88" t="s">
         <v>13</v>
       </c>
@@ -5129,6 +5463,10 @@
       <c r="G89" t="s">
         <v>22</v>
       </c>
+      <c r="H89" s="8">
+        <f>VLOOKUP(G89,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I89" t="s">
         <v>23</v>
       </c>
@@ -5162,6 +5500,10 @@
       <c r="G90" t="s">
         <v>28</v>
       </c>
+      <c r="H90" s="8">
+        <f>VLOOKUP(G90,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I90" t="s">
         <v>245</v>
       </c>
@@ -5195,6 +5537,10 @@
       <c r="G91" t="s">
         <v>22</v>
       </c>
+      <c r="H91" s="8">
+        <f>VLOOKUP(G91,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I91" t="s">
         <v>29</v>
       </c>
@@ -5228,6 +5574,10 @@
       <c r="G92" t="s">
         <v>648</v>
       </c>
+      <c r="H92" s="8">
+        <f>VLOOKUP(G92,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I92" t="s">
         <v>53</v>
       </c>
@@ -5261,6 +5611,10 @@
       <c r="G93" t="s">
         <v>22</v>
       </c>
+      <c r="H93" s="8">
+        <f>VLOOKUP(G93,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I93" t="s">
         <v>13</v>
       </c>
@@ -5291,6 +5645,10 @@
       <c r="G94" t="s">
         <v>228</v>
       </c>
+      <c r="H94" s="8">
+        <f>VLOOKUP(G94,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I94" t="s">
         <v>13</v>
       </c>
@@ -5321,6 +5679,10 @@
       <c r="G95" t="s">
         <v>12</v>
       </c>
+      <c r="H95" s="8">
+        <f>VLOOKUP(G95,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I95" t="s">
         <v>13</v>
       </c>
@@ -5354,6 +5716,10 @@
       <c r="G96" t="s">
         <v>163</v>
       </c>
+      <c r="H96" s="8">
+        <f>VLOOKUP(G96,Fees!$A$2:$B$24,2,0)</f>
+        <v>42</v>
+      </c>
       <c r="I96" t="s">
         <v>13</v>
       </c>
@@ -5387,6 +5753,10 @@
       <c r="G97" t="s">
         <v>12</v>
       </c>
+      <c r="H97" s="8">
+        <f>VLOOKUP(G97,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I97" t="s">
         <v>53</v>
       </c>
@@ -5420,6 +5790,10 @@
       <c r="G98" t="s">
         <v>22</v>
       </c>
+      <c r="H98" s="8">
+        <f>VLOOKUP(G98,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I98" t="s">
         <v>23</v>
       </c>
@@ -5453,6 +5827,10 @@
       <c r="G99" t="s">
         <v>119</v>
       </c>
+      <c r="H99" s="8">
+        <f>VLOOKUP(G99,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I99" t="s">
         <v>53</v>
       </c>
@@ -5486,6 +5864,10 @@
       <c r="G100" t="s">
         <v>188</v>
       </c>
+      <c r="H100" s="8">
+        <f>VLOOKUP(G100,Fees!$A$2:$B$24,2,0)</f>
+        <v>68</v>
+      </c>
       <c r="I100" t="s">
         <v>44</v>
       </c>
@@ -5519,6 +5901,10 @@
       <c r="G101" t="s">
         <v>34</v>
       </c>
+      <c r="H101" s="8">
+        <f>VLOOKUP(G101,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I101" t="s">
         <v>13</v>
       </c>
@@ -5549,6 +5935,10 @@
       <c r="G102" t="s">
         <v>91</v>
       </c>
+      <c r="H102" s="8">
+        <f>VLOOKUP(G102,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I102" t="s">
         <v>53</v>
       </c>
@@ -5579,6 +5969,10 @@
       <c r="G103" t="s">
         <v>163</v>
       </c>
+      <c r="H103" s="8">
+        <f>VLOOKUP(G103,Fees!$A$2:$B$24,2,0)</f>
+        <v>42</v>
+      </c>
       <c r="I103" t="s">
         <v>13</v>
       </c>
@@ -5609,6 +6003,10 @@
       <c r="G104" t="s">
         <v>650</v>
       </c>
+      <c r="H104" s="8">
+        <f>VLOOKUP(G104,Fees!$A$2:$B$24,2,0)</f>
+        <v>25</v>
+      </c>
       <c r="I104" t="s">
         <v>208</v>
       </c>
@@ -5642,6 +6040,10 @@
       <c r="G105" t="s">
         <v>22</v>
       </c>
+      <c r="H105" s="8">
+        <f>VLOOKUP(G105,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I105" t="s">
         <v>29</v>
       </c>
@@ -5672,6 +6074,10 @@
       <c r="G106" t="s">
         <v>228</v>
       </c>
+      <c r="H106" s="8">
+        <f>VLOOKUP(G106,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I106" t="s">
         <v>13</v>
       </c>
@@ -5705,6 +6111,10 @@
       <c r="G107" t="s">
         <v>119</v>
       </c>
+      <c r="H107" s="8">
+        <f>VLOOKUP(G107,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I107" t="s">
         <v>53</v>
       </c>
@@ -5738,6 +6148,10 @@
       <c r="G108" t="s">
         <v>648</v>
       </c>
+      <c r="H108" s="8">
+        <f>VLOOKUP(G108,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I108" t="s">
         <v>13</v>
       </c>
@@ -5768,6 +6182,10 @@
       <c r="G109" t="s">
         <v>119</v>
       </c>
+      <c r="H109" s="8">
+        <f>VLOOKUP(G109,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I109" t="s">
         <v>13</v>
       </c>
@@ -5798,6 +6216,10 @@
       <c r="G110" t="s">
         <v>22</v>
       </c>
+      <c r="H110" s="8">
+        <f>VLOOKUP(G110,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I110" t="s">
         <v>53</v>
       </c>
@@ -5828,6 +6250,10 @@
       <c r="G111" t="s">
         <v>647</v>
       </c>
+      <c r="H111" s="8">
+        <f>VLOOKUP(G111,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I111" t="s">
         <v>13</v>
       </c>
@@ -5858,6 +6284,10 @@
       <c r="G112" t="s">
         <v>43</v>
       </c>
+      <c r="H112" s="8">
+        <f>VLOOKUP(G112,Fees!$A$2:$B$24,2,0)</f>
+        <v>75</v>
+      </c>
       <c r="I112" t="s">
         <v>291</v>
       </c>
@@ -5891,6 +6321,10 @@
       <c r="G113" t="s">
         <v>22</v>
       </c>
+      <c r="H113" s="8">
+        <f>VLOOKUP(G113,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I113" t="s">
         <v>53</v>
       </c>
@@ -5924,6 +6358,10 @@
       <c r="G114" t="s">
         <v>22</v>
       </c>
+      <c r="H114" s="8">
+        <f>VLOOKUP(G114,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I114" t="s">
         <v>23</v>
       </c>
@@ -5957,6 +6395,10 @@
       <c r="G115" t="s">
         <v>34</v>
       </c>
+      <c r="H115" s="8">
+        <f>VLOOKUP(G115,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I115" t="s">
         <v>13</v>
       </c>
@@ -5990,6 +6432,10 @@
       <c r="G116" t="s">
         <v>119</v>
       </c>
+      <c r="H116" s="8">
+        <f>VLOOKUP(G116,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I116" t="s">
         <v>13</v>
       </c>
@@ -6020,6 +6466,10 @@
       <c r="G117" t="s">
         <v>95</v>
       </c>
+      <c r="H117" s="8">
+        <f>VLOOKUP(G117,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I117" t="s">
         <v>13</v>
       </c>
@@ -6050,6 +6500,10 @@
       <c r="G118" t="s">
         <v>91</v>
       </c>
+      <c r="H118" s="8">
+        <f>VLOOKUP(G118,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I118" t="s">
         <v>13</v>
       </c>
@@ -6080,6 +6534,10 @@
       <c r="G119" t="s">
         <v>228</v>
       </c>
+      <c r="H119" s="8">
+        <f>VLOOKUP(G119,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I119" t="s">
         <v>53</v>
       </c>
@@ -6110,6 +6568,10 @@
       <c r="G120" t="s">
         <v>18</v>
       </c>
+      <c r="H120" s="8">
+        <f>VLOOKUP(G120,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I120" t="s">
         <v>29</v>
       </c>
@@ -6140,6 +6602,10 @@
       <c r="G121" t="s">
         <v>648</v>
       </c>
+      <c r="H121" s="8">
+        <f>VLOOKUP(G121,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I121" t="s">
         <v>23</v>
       </c>
@@ -6170,6 +6636,10 @@
       <c r="G122" t="s">
         <v>28</v>
       </c>
+      <c r="H122" s="8">
+        <f>VLOOKUP(G122,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I122" t="s">
         <v>208</v>
       </c>
@@ -6200,6 +6670,10 @@
       <c r="G123" t="s">
         <v>169</v>
       </c>
+      <c r="H123" s="8">
+        <f>VLOOKUP(G123,Fees!$A$2:$B$24,2,0)</f>
+        <v>23</v>
+      </c>
       <c r="I123" t="s">
         <v>53</v>
       </c>
@@ -6230,6 +6704,10 @@
       <c r="G124" t="s">
         <v>39</v>
       </c>
+      <c r="H124" s="8">
+        <f>VLOOKUP(G124,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I124" t="s">
         <v>53</v>
       </c>
@@ -6260,6 +6738,10 @@
       <c r="G125" t="s">
         <v>647</v>
       </c>
+      <c r="H125" s="8">
+        <f>VLOOKUP(G125,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I125" t="s">
         <v>29</v>
       </c>
@@ -6290,6 +6772,10 @@
       <c r="G126" t="s">
         <v>648</v>
       </c>
+      <c r="H126" s="8">
+        <f>VLOOKUP(G126,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I126" t="s">
         <v>53</v>
       </c>
@@ -6323,6 +6809,10 @@
       <c r="G127" t="s">
         <v>648</v>
       </c>
+      <c r="H127" s="8">
+        <f>VLOOKUP(G127,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I127" t="s">
         <v>29</v>
       </c>
@@ -6353,6 +6843,10 @@
       <c r="G128" t="s">
         <v>18</v>
       </c>
+      <c r="H128" s="8">
+        <f>VLOOKUP(G128,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I128" t="s">
         <v>23</v>
       </c>
@@ -6386,6 +6880,10 @@
       <c r="G129" t="s">
         <v>119</v>
       </c>
+      <c r="H129" s="8">
+        <f>VLOOKUP(G129,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I129" t="s">
         <v>23</v>
       </c>
@@ -6419,6 +6917,10 @@
       <c r="G130" t="s">
         <v>647</v>
       </c>
+      <c r="H130" s="8">
+        <f>VLOOKUP(G130,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I130" t="s">
         <v>13</v>
       </c>
@@ -6449,6 +6951,10 @@
       <c r="G131" t="s">
         <v>91</v>
       </c>
+      <c r="H131" s="8">
+        <f>VLOOKUP(G131,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I131" t="s">
         <v>333</v>
       </c>
@@ -6482,6 +6988,10 @@
       <c r="G132" t="s">
         <v>647</v>
       </c>
+      <c r="H132" s="8">
+        <f>VLOOKUP(G132,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I132" t="s">
         <v>13</v>
       </c>
@@ -6515,6 +7025,10 @@
       <c r="G133" t="s">
         <v>28</v>
       </c>
+      <c r="H133" s="8">
+        <f>VLOOKUP(G133,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I133" t="s">
         <v>338</v>
       </c>
@@ -6545,6 +7059,10 @@
       <c r="G134" t="s">
         <v>18</v>
       </c>
+      <c r="H134" s="8">
+        <f>VLOOKUP(G134,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I134" t="s">
         <v>35</v>
       </c>
@@ -6575,6 +7093,10 @@
       <c r="G135" t="s">
         <v>22</v>
       </c>
+      <c r="H135" s="8">
+        <f>VLOOKUP(G135,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I135" t="s">
         <v>13</v>
       </c>
@@ -6605,6 +7127,10 @@
       <c r="G136" t="s">
         <v>34</v>
       </c>
+      <c r="H136" s="8">
+        <f>VLOOKUP(G136,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I136" t="s">
         <v>13</v>
       </c>
@@ -6638,6 +7164,10 @@
       <c r="G137" t="s">
         <v>22</v>
       </c>
+      <c r="H137" s="8">
+        <f>VLOOKUP(G137,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I137" t="s">
         <v>13</v>
       </c>
@@ -6671,6 +7201,10 @@
       <c r="G138" t="s">
         <v>28</v>
       </c>
+      <c r="H138" s="8">
+        <f>VLOOKUP(G138,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I138" t="s">
         <v>35</v>
       </c>
@@ -6704,6 +7238,10 @@
       <c r="G139" t="s">
         <v>647</v>
       </c>
+      <c r="H139" s="8">
+        <f>VLOOKUP(G139,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I139" t="s">
         <v>23</v>
       </c>
@@ -6734,6 +7272,10 @@
       <c r="G140" t="s">
         <v>28</v>
       </c>
+      <c r="H140" s="8">
+        <f>VLOOKUP(G140,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I140" t="s">
         <v>35</v>
       </c>
@@ -6767,6 +7309,10 @@
       <c r="G141" t="s">
         <v>22</v>
       </c>
+      <c r="H141" s="8">
+        <f>VLOOKUP(G141,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I141" t="s">
         <v>23</v>
       </c>
@@ -6800,6 +7346,10 @@
       <c r="G142" t="s">
         <v>39</v>
       </c>
+      <c r="H142" s="8">
+        <f>VLOOKUP(G142,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I142" t="s">
         <v>53</v>
       </c>
@@ -6830,6 +7380,10 @@
       <c r="G143" t="s">
         <v>91</v>
       </c>
+      <c r="H143" s="8">
+        <f>VLOOKUP(G143,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I143" t="s">
         <v>53</v>
       </c>
@@ -6860,6 +7414,10 @@
       <c r="G144" t="s">
         <v>91</v>
       </c>
+      <c r="H144" s="8">
+        <f>VLOOKUP(G144,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I144" t="s">
         <v>29</v>
       </c>
@@ -6890,6 +7448,10 @@
       <c r="G145" t="s">
         <v>22</v>
       </c>
+      <c r="H145" s="8">
+        <f>VLOOKUP(G145,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I145" t="s">
         <v>53</v>
       </c>
@@ -6920,6 +7482,10 @@
       <c r="G146" t="s">
         <v>648</v>
       </c>
+      <c r="H146" s="8">
+        <f>VLOOKUP(G146,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I146" t="s">
         <v>13</v>
       </c>
@@ -6950,6 +7516,10 @@
       <c r="G147" t="s">
         <v>22</v>
       </c>
+      <c r="H147" s="8">
+        <f>VLOOKUP(G147,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I147" t="s">
         <v>53</v>
       </c>
@@ -6983,6 +7553,10 @@
       <c r="G148" t="s">
         <v>28</v>
       </c>
+      <c r="H148" s="8">
+        <f>VLOOKUP(G148,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I148" t="s">
         <v>109</v>
       </c>
@@ -7016,6 +7590,10 @@
       <c r="G149" t="s">
         <v>22</v>
       </c>
+      <c r="H149" s="8">
+        <f>VLOOKUP(G149,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I149" t="s">
         <v>53</v>
       </c>
@@ -7049,6 +7627,10 @@
       <c r="G150" t="s">
         <v>184</v>
       </c>
+      <c r="H150" s="8">
+        <f>VLOOKUP(G150,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I150" t="s">
         <v>13</v>
       </c>
@@ -7082,6 +7664,10 @@
       <c r="G151" t="s">
         <v>22</v>
       </c>
+      <c r="H151" s="8">
+        <f>VLOOKUP(G151,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I151" t="s">
         <v>13</v>
       </c>
@@ -7115,6 +7701,10 @@
       <c r="G152" t="s">
         <v>184</v>
       </c>
+      <c r="H152" s="8">
+        <f>VLOOKUP(G152,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I152" t="s">
         <v>23</v>
       </c>
@@ -7148,6 +7738,10 @@
       <c r="G153" t="s">
         <v>119</v>
       </c>
+      <c r="H153" s="8">
+        <f>VLOOKUP(G153,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I153" t="s">
         <v>23</v>
       </c>
@@ -7181,6 +7775,10 @@
       <c r="G154" t="s">
         <v>22</v>
       </c>
+      <c r="H154" s="8">
+        <f>VLOOKUP(G154,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I154" t="s">
         <v>13</v>
       </c>
@@ -7214,6 +7812,10 @@
       <c r="G155" t="s">
         <v>34</v>
       </c>
+      <c r="H155" s="8">
+        <f>VLOOKUP(G155,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I155" t="s">
         <v>53</v>
       </c>
@@ -7247,6 +7849,10 @@
       <c r="G156" t="s">
         <v>22</v>
       </c>
+      <c r="H156" s="8">
+        <f>VLOOKUP(G156,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I156" t="s">
         <v>53</v>
       </c>
@@ -7280,6 +7886,10 @@
       <c r="G157" t="s">
         <v>648</v>
       </c>
+      <c r="H157" s="8">
+        <f>VLOOKUP(G157,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I157" t="s">
         <v>29</v>
       </c>
@@ -7310,6 +7920,10 @@
       <c r="G158" t="s">
         <v>647</v>
       </c>
+      <c r="H158" s="8">
+        <f>VLOOKUP(G158,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I158" t="s">
         <v>13</v>
       </c>
@@ -7340,6 +7954,10 @@
       <c r="G159" t="s">
         <v>649</v>
       </c>
+      <c r="H159" s="8">
+        <f>VLOOKUP(G159,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I159" t="s">
         <v>23</v>
       </c>
@@ -7370,6 +7988,10 @@
       <c r="G160" t="s">
         <v>648</v>
       </c>
+      <c r="H160" s="8">
+        <f>VLOOKUP(G160,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I160" t="s">
         <v>13</v>
       </c>
@@ -7400,6 +8022,10 @@
       <c r="G161" t="s">
         <v>22</v>
       </c>
+      <c r="H161" s="8">
+        <f>VLOOKUP(G161,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I161" t="s">
         <v>13</v>
       </c>
@@ -7430,6 +8056,10 @@
       <c r="G162" t="s">
         <v>18</v>
       </c>
+      <c r="H162" s="8">
+        <f>VLOOKUP(G162,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I162" t="s">
         <v>13</v>
       </c>
@@ -7460,6 +8090,10 @@
       <c r="G163" t="s">
         <v>645</v>
       </c>
+      <c r="H163" s="8">
+        <f>VLOOKUP(G163,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
+      </c>
       <c r="I163" t="s">
         <v>35</v>
       </c>
@@ -7490,6 +8124,10 @@
       <c r="G164" t="s">
         <v>188</v>
       </c>
+      <c r="H164" s="8">
+        <f>VLOOKUP(G164,Fees!$A$2:$B$24,2,0)</f>
+        <v>68</v>
+      </c>
       <c r="I164" t="s">
         <v>44</v>
       </c>
@@ -7520,6 +8158,10 @@
       <c r="G165" t="s">
         <v>22</v>
       </c>
+      <c r="H165" s="8">
+        <f>VLOOKUP(G165,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I165" t="s">
         <v>23</v>
       </c>
@@ -7550,6 +8192,10 @@
       <c r="G166" t="s">
         <v>22</v>
       </c>
+      <c r="H166" s="8">
+        <f>VLOOKUP(G166,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I166" t="s">
         <v>23</v>
       </c>
@@ -7580,6 +8226,10 @@
       <c r="G167" t="s">
         <v>22</v>
       </c>
+      <c r="H167" s="8">
+        <f>VLOOKUP(G167,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I167" t="s">
         <v>13</v>
       </c>
@@ -7610,6 +8260,10 @@
       <c r="G168" t="s">
         <v>95</v>
       </c>
+      <c r="H168" s="8">
+        <f>VLOOKUP(G168,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I168" t="s">
         <v>109</v>
       </c>
@@ -7640,6 +8294,10 @@
       <c r="G169" t="s">
         <v>34</v>
       </c>
+      <c r="H169" s="8">
+        <f>VLOOKUP(G169,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I169" t="s">
         <v>23</v>
       </c>
@@ -7670,6 +8328,10 @@
       <c r="G170" t="s">
         <v>22</v>
       </c>
+      <c r="H170" s="8">
+        <f>VLOOKUP(G170,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I170" t="s">
         <v>53</v>
       </c>
@@ -7703,6 +8365,10 @@
       <c r="G171" t="s">
         <v>22</v>
       </c>
+      <c r="H171" s="8">
+        <f>VLOOKUP(G171,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I171" t="s">
         <v>13</v>
       </c>
@@ -7736,6 +8402,10 @@
       <c r="G172" t="s">
         <v>28</v>
       </c>
+      <c r="H172" s="8">
+        <f>VLOOKUP(G172,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I172" t="s">
         <v>13</v>
       </c>
@@ -7769,6 +8439,10 @@
       <c r="G173" t="s">
         <v>18</v>
       </c>
+      <c r="H173" s="8">
+        <f>VLOOKUP(G173,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I173" t="s">
         <v>53</v>
       </c>
@@ -7799,6 +8473,10 @@
       <c r="G174" t="s">
         <v>22</v>
       </c>
+      <c r="H174" s="8">
+        <f>VLOOKUP(G174,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I174" t="s">
         <v>53</v>
       </c>
@@ -7829,6 +8507,10 @@
       <c r="G175" t="s">
         <v>22</v>
       </c>
+      <c r="H175" s="8">
+        <f>VLOOKUP(G175,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I175" t="s">
         <v>23</v>
       </c>
@@ -7859,6 +8541,10 @@
       <c r="G176" t="s">
         <v>22</v>
       </c>
+      <c r="H176" s="8">
+        <f>VLOOKUP(G176,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I176" t="s">
         <v>23</v>
       </c>
@@ -7889,6 +8575,10 @@
       <c r="G177" t="s">
         <v>22</v>
       </c>
+      <c r="H177" s="8">
+        <f>VLOOKUP(G177,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I177" t="s">
         <v>53</v>
       </c>
@@ -7919,6 +8609,10 @@
       <c r="G178" t="s">
         <v>12</v>
       </c>
+      <c r="H178" s="8">
+        <f>VLOOKUP(G178,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I178" t="s">
         <v>13</v>
       </c>
@@ -7949,6 +8643,10 @@
       <c r="G179" t="s">
         <v>645</v>
       </c>
+      <c r="H179" s="8">
+        <f>VLOOKUP(G179,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
+      </c>
       <c r="I179" t="s">
         <v>23</v>
       </c>
@@ -7979,6 +8677,10 @@
       <c r="G180" t="s">
         <v>39</v>
       </c>
+      <c r="H180" s="8">
+        <f>VLOOKUP(G180,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I180" t="s">
         <v>13</v>
       </c>
@@ -8012,6 +8714,10 @@
       <c r="G181" t="s">
         <v>22</v>
       </c>
+      <c r="H181" s="8">
+        <f>VLOOKUP(G181,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I181" t="s">
         <v>13</v>
       </c>
@@ -8042,6 +8748,10 @@
       <c r="G182" t="s">
         <v>647</v>
       </c>
+      <c r="H182" s="8">
+        <f>VLOOKUP(G182,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I182" t="s">
         <v>13</v>
       </c>
@@ -8072,6 +8782,10 @@
       <c r="G183" t="s">
         <v>34</v>
       </c>
+      <c r="H183" s="8">
+        <f>VLOOKUP(G183,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I183" t="s">
         <v>13</v>
       </c>
@@ -8105,6 +8819,10 @@
       <c r="G184" t="s">
         <v>228</v>
       </c>
+      <c r="H184" s="8">
+        <f>VLOOKUP(G184,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I184" t="s">
         <v>29</v>
       </c>
@@ -8135,6 +8853,10 @@
       <c r="G185" t="s">
         <v>68</v>
       </c>
+      <c r="H185" s="8">
+        <f>VLOOKUP(G185,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I185" t="s">
         <v>13</v>
       </c>
@@ -8165,6 +8887,10 @@
       <c r="G186" t="s">
         <v>28</v>
       </c>
+      <c r="H186" s="8">
+        <f>VLOOKUP(G186,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I186" t="s">
         <v>13</v>
       </c>
@@ -8195,6 +8921,10 @@
       <c r="G187" t="s">
         <v>43</v>
       </c>
+      <c r="H187" s="8">
+        <f>VLOOKUP(G187,Fees!$A$2:$B$24,2,0)</f>
+        <v>75</v>
+      </c>
       <c r="I187" t="s">
         <v>44</v>
       </c>
@@ -8225,6 +8955,10 @@
       <c r="G188" t="s">
         <v>119</v>
       </c>
+      <c r="H188" s="8">
+        <f>VLOOKUP(G188,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I188" t="s">
         <v>23</v>
       </c>
@@ -8258,6 +8992,10 @@
       <c r="G189" t="s">
         <v>34</v>
       </c>
+      <c r="H189" s="8">
+        <f>VLOOKUP(G189,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I189" t="s">
         <v>35</v>
       </c>
@@ -8288,6 +9026,10 @@
       <c r="G190" t="s">
         <v>91</v>
       </c>
+      <c r="H190" s="8">
+        <f>VLOOKUP(G190,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I190" t="s">
         <v>29</v>
       </c>
@@ -8321,6 +9063,10 @@
       <c r="G191" t="s">
         <v>18</v>
       </c>
+      <c r="H191" s="8">
+        <f>VLOOKUP(G191,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I191" t="s">
         <v>13</v>
       </c>
@@ -8354,6 +9100,10 @@
       <c r="G192" t="s">
         <v>22</v>
       </c>
+      <c r="H192" s="8">
+        <f>VLOOKUP(G192,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I192" t="s">
         <v>29</v>
       </c>
@@ -8387,6 +9137,10 @@
       <c r="G193" t="s">
         <v>91</v>
       </c>
+      <c r="H193" s="8">
+        <f>VLOOKUP(G193,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I193" t="s">
         <v>35</v>
       </c>
@@ -8420,6 +9174,10 @@
       <c r="G194" t="s">
         <v>34</v>
       </c>
+      <c r="H194" s="8">
+        <f>VLOOKUP(G194,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I194" t="s">
         <v>13</v>
       </c>
@@ -8453,6 +9211,10 @@
       <c r="G195" t="s">
         <v>119</v>
       </c>
+      <c r="H195" s="8">
+        <f>VLOOKUP(G195,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I195" t="s">
         <v>13</v>
       </c>
@@ -8483,6 +9245,10 @@
       <c r="G196" t="s">
         <v>22</v>
       </c>
+      <c r="H196" s="8">
+        <f>VLOOKUP(G196,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I196" t="s">
         <v>13</v>
       </c>
@@ -8516,6 +9282,10 @@
       <c r="G197" t="s">
         <v>646</v>
       </c>
+      <c r="H197" s="8">
+        <f>VLOOKUP(G197,Fees!$A$2:$B$24,2,0)</f>
+        <v>60</v>
+      </c>
       <c r="I197" t="s">
         <v>13</v>
       </c>
@@ -8546,6 +9316,10 @@
       <c r="G198" t="s">
         <v>39</v>
       </c>
+      <c r="H198" s="8">
+        <f>VLOOKUP(G198,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I198" t="s">
         <v>53</v>
       </c>
@@ -8576,6 +9350,10 @@
       <c r="G199" t="s">
         <v>34</v>
       </c>
+      <c r="H199" s="8">
+        <f>VLOOKUP(G199,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I199" t="s">
         <v>35</v>
       </c>
@@ -8606,6 +9384,10 @@
       <c r="G200" t="s">
         <v>91</v>
       </c>
+      <c r="H200" s="8">
+        <f>VLOOKUP(G200,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I200" t="s">
         <v>35</v>
       </c>
@@ -8636,6 +9418,10 @@
       <c r="G201" t="s">
         <v>22</v>
       </c>
+      <c r="H201" s="8">
+        <f>VLOOKUP(G201,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I201" t="s">
         <v>23</v>
       </c>
@@ -8669,6 +9455,10 @@
       <c r="G202" t="s">
         <v>22</v>
       </c>
+      <c r="H202" s="8">
+        <f>VLOOKUP(G202,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I202" t="s">
         <v>23</v>
       </c>
@@ -8699,6 +9489,10 @@
       <c r="G203" t="s">
         <v>95</v>
       </c>
+      <c r="H203" s="8">
+        <f>VLOOKUP(G203,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I203" t="s">
         <v>13</v>
       </c>
@@ -8729,6 +9523,10 @@
       <c r="G204" t="s">
         <v>645</v>
       </c>
+      <c r="H204" s="8">
+        <f>VLOOKUP(G204,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
+      </c>
       <c r="I204" t="s">
         <v>35</v>
       </c>
@@ -8759,6 +9557,10 @@
       <c r="G205" t="s">
         <v>91</v>
       </c>
+      <c r="H205" s="8">
+        <f>VLOOKUP(G205,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I205" t="s">
         <v>53</v>
       </c>
@@ -8789,6 +9591,10 @@
       <c r="G206" t="s">
         <v>184</v>
       </c>
+      <c r="H206" s="8">
+        <f>VLOOKUP(G206,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I206" t="s">
         <v>13</v>
       </c>
@@ -8819,6 +9625,10 @@
       <c r="G207" t="s">
         <v>22</v>
       </c>
+      <c r="H207" s="8">
+        <f>VLOOKUP(G207,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I207" t="s">
         <v>23</v>
       </c>
@@ -8849,6 +9659,10 @@
       <c r="G208" t="s">
         <v>34</v>
       </c>
+      <c r="H208" s="8">
+        <f>VLOOKUP(G208,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I208" t="s">
         <v>53</v>
       </c>
@@ -8879,6 +9693,10 @@
       <c r="G209" t="s">
         <v>34</v>
       </c>
+      <c r="H209" s="8">
+        <f>VLOOKUP(G209,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I209" t="s">
         <v>35</v>
       </c>
@@ -8909,6 +9727,10 @@
       <c r="G210" t="s">
         <v>91</v>
       </c>
+      <c r="H210" s="8">
+        <f>VLOOKUP(G210,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I210" t="s">
         <v>53</v>
       </c>
@@ -8939,6 +9761,10 @@
       <c r="G211" t="s">
         <v>228</v>
       </c>
+      <c r="H211" s="8">
+        <f>VLOOKUP(G211,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I211" t="s">
         <v>23</v>
       </c>
@@ -8972,6 +9798,10 @@
       <c r="G212" t="s">
         <v>647</v>
       </c>
+      <c r="H212" s="8">
+        <f>VLOOKUP(G212,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I212" t="s">
         <v>23</v>
       </c>
@@ -9002,6 +9832,10 @@
       <c r="G213" t="s">
         <v>22</v>
       </c>
+      <c r="H213" s="8">
+        <f>VLOOKUP(G213,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I213" t="s">
         <v>23</v>
       </c>
@@ -9032,6 +9866,10 @@
       <c r="G214" t="s">
         <v>91</v>
       </c>
+      <c r="H214" s="8">
+        <f>VLOOKUP(G214,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I214" t="s">
         <v>53</v>
       </c>
@@ -9062,6 +9900,10 @@
       <c r="G215" t="s">
         <v>22</v>
       </c>
+      <c r="H215" s="8">
+        <f>VLOOKUP(G215,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I215" t="s">
         <v>208</v>
       </c>
@@ -9092,6 +9934,10 @@
       <c r="G216" t="s">
         <v>647</v>
       </c>
+      <c r="H216" s="8">
+        <f>VLOOKUP(G216,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I216" t="s">
         <v>53</v>
       </c>
@@ -9122,6 +9968,10 @@
       <c r="G217" t="s">
         <v>647</v>
       </c>
+      <c r="H217" s="8">
+        <f>VLOOKUP(G217,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I217" t="s">
         <v>53</v>
       </c>
@@ -9152,6 +10002,10 @@
       <c r="G218" t="s">
         <v>22</v>
       </c>
+      <c r="H218" s="8">
+        <f>VLOOKUP(G218,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I218" t="s">
         <v>23</v>
       </c>
@@ -9182,6 +10036,10 @@
       <c r="G219" t="s">
         <v>34</v>
       </c>
+      <c r="H219" s="8">
+        <f>VLOOKUP(G219,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I219" t="s">
         <v>13</v>
       </c>
@@ -9212,6 +10070,10 @@
       <c r="G220" t="s">
         <v>649</v>
       </c>
+      <c r="H220" s="8">
+        <f>VLOOKUP(G220,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I220" t="s">
         <v>23</v>
       </c>
@@ -9242,6 +10104,10 @@
       <c r="G221" t="s">
         <v>34</v>
       </c>
+      <c r="H221" s="8">
+        <f>VLOOKUP(G221,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I221" t="s">
         <v>23</v>
       </c>
@@ -9272,6 +10138,10 @@
       <c r="G222" t="s">
         <v>28</v>
       </c>
+      <c r="H222" s="8">
+        <f>VLOOKUP(G222,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I222" t="s">
         <v>338</v>
       </c>
@@ -9302,6 +10172,10 @@
       <c r="G223" t="s">
         <v>184</v>
       </c>
+      <c r="H223" s="8">
+        <f>VLOOKUP(G223,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I223" t="s">
         <v>35</v>
       </c>
@@ -9332,6 +10206,10 @@
       <c r="G224" t="s">
         <v>18</v>
       </c>
+      <c r="H224" s="8">
+        <f>VLOOKUP(G224,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I224" t="s">
         <v>53</v>
       </c>
@@ -9365,6 +10243,10 @@
       <c r="G225" t="s">
         <v>18</v>
       </c>
+      <c r="H225" s="8">
+        <f>VLOOKUP(G225,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I225" t="s">
         <v>23</v>
       </c>
@@ -9398,6 +10280,10 @@
       <c r="G226" t="s">
         <v>91</v>
       </c>
+      <c r="H226" s="8">
+        <f>VLOOKUP(G226,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I226" t="s">
         <v>35</v>
       </c>
@@ -9431,6 +10317,10 @@
       <c r="G227" t="s">
         <v>28</v>
       </c>
+      <c r="H227" s="8">
+        <f>VLOOKUP(G227,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I227" t="s">
         <v>53</v>
       </c>
@@ -9464,6 +10354,10 @@
       <c r="G228" t="s">
         <v>12</v>
       </c>
+      <c r="H228" s="8">
+        <f>VLOOKUP(G228,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I228" t="s">
         <v>13</v>
       </c>
@@ -9494,6 +10388,10 @@
       <c r="G229" t="s">
         <v>119</v>
       </c>
+      <c r="H229" s="8">
+        <f>VLOOKUP(G229,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I229" t="s">
         <v>13</v>
       </c>
@@ -9527,6 +10425,10 @@
       <c r="G230" t="s">
         <v>649</v>
       </c>
+      <c r="H230" s="8">
+        <f>VLOOKUP(G230,Fees!$A$2:$B$24,2,0)</f>
+        <v>64</v>
+      </c>
       <c r="I230" t="s">
         <v>208</v>
       </c>
@@ -9560,6 +10462,10 @@
       <c r="G231" t="s">
         <v>22</v>
       </c>
+      <c r="H231" s="8">
+        <f>VLOOKUP(G231,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I231" t="s">
         <v>13</v>
       </c>
@@ -9590,6 +10496,10 @@
       <c r="G232" t="s">
         <v>34</v>
       </c>
+      <c r="H232" s="8">
+        <f>VLOOKUP(G232,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I232" t="s">
         <v>53</v>
       </c>
@@ -9620,6 +10530,10 @@
       <c r="G233" t="s">
         <v>188</v>
       </c>
+      <c r="H233" s="8">
+        <f>VLOOKUP(G233,Fees!$A$2:$B$24,2,0)</f>
+        <v>68</v>
+      </c>
       <c r="I233" t="s">
         <v>44</v>
       </c>
@@ -9650,6 +10564,10 @@
       <c r="G234" t="s">
         <v>228</v>
       </c>
+      <c r="H234" s="8">
+        <f>VLOOKUP(G234,Fees!$A$2:$B$24,2,0)</f>
+        <v>26</v>
+      </c>
       <c r="I234" t="s">
         <v>53</v>
       </c>
@@ -9680,6 +10598,10 @@
       <c r="G235" t="s">
         <v>22</v>
       </c>
+      <c r="H235" s="8">
+        <f>VLOOKUP(G235,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I235" t="s">
         <v>29</v>
       </c>
@@ -9713,6 +10635,10 @@
       <c r="G236" t="s">
         <v>34</v>
       </c>
+      <c r="H236" s="8">
+        <f>VLOOKUP(G236,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I236" t="s">
         <v>13</v>
       </c>
@@ -9746,6 +10672,10 @@
       <c r="G237" t="s">
         <v>22</v>
       </c>
+      <c r="H237" s="8">
+        <f>VLOOKUP(G237,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I237" t="s">
         <v>53</v>
       </c>
@@ -9776,6 +10706,10 @@
       <c r="G238" t="s">
         <v>646</v>
       </c>
+      <c r="H238" s="8">
+        <f>VLOOKUP(G238,Fees!$A$2:$B$24,2,0)</f>
+        <v>60</v>
+      </c>
       <c r="I238" t="s">
         <v>13</v>
       </c>
@@ -9809,6 +10743,10 @@
       <c r="G239" t="s">
         <v>645</v>
       </c>
+      <c r="H239" s="8">
+        <f>VLOOKUP(G239,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
+      </c>
       <c r="I239" t="s">
         <v>23</v>
       </c>
@@ -9842,6 +10780,10 @@
       <c r="G240" t="s">
         <v>22</v>
       </c>
+      <c r="H240" s="8">
+        <f>VLOOKUP(G240,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I240" t="s">
         <v>13</v>
       </c>
@@ -9875,6 +10817,10 @@
       <c r="G241" t="s">
         <v>646</v>
       </c>
+      <c r="H241" s="8">
+        <f>VLOOKUP(G241,Fees!$A$2:$B$24,2,0)</f>
+        <v>60</v>
+      </c>
       <c r="I241" t="s">
         <v>53</v>
       </c>
@@ -9908,6 +10854,10 @@
       <c r="G242" t="s">
         <v>12</v>
       </c>
+      <c r="H242" s="8">
+        <f>VLOOKUP(G242,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I242" t="s">
         <v>13</v>
       </c>
@@ -9938,6 +10888,10 @@
       <c r="G243" t="s">
         <v>34</v>
       </c>
+      <c r="H243" s="8">
+        <f>VLOOKUP(G243,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I243" t="s">
         <v>13</v>
       </c>
@@ -9968,6 +10922,10 @@
       <c r="G244" t="s">
         <v>34</v>
       </c>
+      <c r="H244" s="8">
+        <f>VLOOKUP(G244,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I244" t="s">
         <v>53</v>
       </c>
@@ -9998,6 +10956,10 @@
       <c r="G245" t="s">
         <v>39</v>
       </c>
+      <c r="H245" s="8">
+        <f>VLOOKUP(G245,Fees!$A$2:$B$24,2,0)</f>
+        <v>81</v>
+      </c>
       <c r="I245" t="s">
         <v>23</v>
       </c>
@@ -10028,6 +10990,10 @@
       <c r="G246" t="s">
         <v>647</v>
       </c>
+      <c r="H246" s="8">
+        <f>VLOOKUP(G246,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I246" t="s">
         <v>53</v>
       </c>
@@ -10058,6 +11024,10 @@
       <c r="G247" t="s">
         <v>648</v>
       </c>
+      <c r="H247" s="8">
+        <f>VLOOKUP(G247,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I247" t="s">
         <v>29</v>
       </c>
@@ -10088,6 +11058,10 @@
       <c r="G248" t="s">
         <v>22</v>
       </c>
+      <c r="H248" s="8">
+        <f>VLOOKUP(G248,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I248" t="s">
         <v>23</v>
       </c>
@@ -10118,6 +11092,10 @@
       <c r="G249" t="s">
         <v>650</v>
       </c>
+      <c r="H249" s="8">
+        <f>VLOOKUP(G249,Fees!$A$2:$B$24,2,0)</f>
+        <v>25</v>
+      </c>
       <c r="I249" t="s">
         <v>13</v>
       </c>
@@ -10148,6 +11126,10 @@
       <c r="G250" t="s">
         <v>91</v>
       </c>
+      <c r="H250" s="8">
+        <f>VLOOKUP(G250,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I250" t="s">
         <v>53</v>
       </c>
@@ -10178,6 +11160,10 @@
       <c r="G251" t="s">
         <v>119</v>
       </c>
+      <c r="H251" s="8">
+        <f>VLOOKUP(G251,Fees!$A$2:$B$24,2,0)</f>
+        <v>41</v>
+      </c>
       <c r="I251" t="s">
         <v>23</v>
       </c>
@@ -10211,6 +11197,10 @@
       <c r="G252" t="s">
         <v>91</v>
       </c>
+      <c r="H252" s="8">
+        <f>VLOOKUP(G252,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I252" t="s">
         <v>23</v>
       </c>
@@ -10241,6 +11231,10 @@
       <c r="G253" t="s">
         <v>22</v>
       </c>
+      <c r="H253" s="8">
+        <f>VLOOKUP(G253,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I253" t="s">
         <v>53</v>
       </c>
@@ -10274,6 +11268,10 @@
       <c r="G254" t="s">
         <v>28</v>
       </c>
+      <c r="H254" s="8">
+        <f>VLOOKUP(G254,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I254" t="s">
         <v>29</v>
       </c>
@@ -10307,6 +11305,10 @@
       <c r="G255" t="s">
         <v>91</v>
       </c>
+      <c r="H255" s="8">
+        <f>VLOOKUP(G255,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I255" t="s">
         <v>13</v>
       </c>
@@ -10340,6 +11342,10 @@
       <c r="G256" t="s">
         <v>95</v>
       </c>
+      <c r="H256" s="8">
+        <f>VLOOKUP(G256,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I256" t="s">
         <v>23</v>
       </c>
@@ -10370,6 +11376,10 @@
       <c r="G257" t="s">
         <v>18</v>
       </c>
+      <c r="H257" s="8">
+        <f>VLOOKUP(G257,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I257" t="s">
         <v>53</v>
       </c>
@@ -10400,6 +11410,10 @@
       <c r="G258" t="s">
         <v>95</v>
       </c>
+      <c r="H258" s="8">
+        <f>VLOOKUP(G258,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I258" t="s">
         <v>29</v>
       </c>
@@ -10430,6 +11444,10 @@
       <c r="G259" t="s">
         <v>22</v>
       </c>
+      <c r="H259" s="8">
+        <f>VLOOKUP(G259,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I259" t="s">
         <v>23</v>
       </c>
@@ -10460,6 +11478,10 @@
       <c r="G260" t="s">
         <v>22</v>
       </c>
+      <c r="H260" s="8">
+        <f>VLOOKUP(G260,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I260" t="s">
         <v>13</v>
       </c>
@@ -10490,6 +11512,10 @@
       <c r="G261" t="s">
         <v>12</v>
       </c>
+      <c r="H261" s="8">
+        <f>VLOOKUP(G261,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I261" t="s">
         <v>53</v>
       </c>
@@ -10523,6 +11549,10 @@
       <c r="G262" t="s">
         <v>184</v>
       </c>
+      <c r="H262" s="8">
+        <f>VLOOKUP(G262,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I262" t="s">
         <v>53</v>
       </c>
@@ -10553,6 +11583,10 @@
       <c r="G263" t="s">
         <v>18</v>
       </c>
+      <c r="H263" s="8">
+        <f>VLOOKUP(G263,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I263" t="s">
         <v>13</v>
       </c>
@@ -10586,6 +11620,10 @@
       <c r="G264" t="s">
         <v>12</v>
       </c>
+      <c r="H264" s="8">
+        <f>VLOOKUP(G264,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I264" t="s">
         <v>23</v>
       </c>
@@ -10616,6 +11654,10 @@
       <c r="G265" t="s">
         <v>95</v>
       </c>
+      <c r="H265" s="8">
+        <f>VLOOKUP(G265,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I265" t="s">
         <v>23</v>
       </c>
@@ -10646,6 +11688,10 @@
       <c r="G266" t="s">
         <v>22</v>
       </c>
+      <c r="H266" s="8">
+        <f>VLOOKUP(G266,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I266" t="s">
         <v>13</v>
       </c>
@@ -10676,6 +11722,10 @@
       <c r="G267" t="s">
         <v>22</v>
       </c>
+      <c r="H267" s="8">
+        <f>VLOOKUP(G267,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I267" t="s">
         <v>13</v>
       </c>
@@ -10709,6 +11759,10 @@
       <c r="G268" t="s">
         <v>184</v>
       </c>
+      <c r="H268" s="8">
+        <f>VLOOKUP(G268,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I268" t="s">
         <v>13</v>
       </c>
@@ -10742,6 +11796,10 @@
       <c r="G269" t="s">
         <v>12</v>
       </c>
+      <c r="H269" s="8">
+        <f>VLOOKUP(G269,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I269" t="s">
         <v>13</v>
       </c>
@@ -10775,6 +11833,10 @@
       <c r="G270" t="s">
         <v>34</v>
       </c>
+      <c r="H270" s="8">
+        <f>VLOOKUP(G270,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I270" t="s">
         <v>13</v>
       </c>
@@ -10805,6 +11867,10 @@
       <c r="G271" t="s">
         <v>68</v>
       </c>
+      <c r="H271" s="8">
+        <f>VLOOKUP(G271,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I271" t="s">
         <v>13</v>
       </c>
@@ -10835,6 +11901,10 @@
       <c r="G272" t="s">
         <v>91</v>
       </c>
+      <c r="H272" s="8">
+        <f>VLOOKUP(G272,Fees!$A$2:$B$24,2,0)</f>
+        <v>85</v>
+      </c>
       <c r="I272" t="s">
         <v>53</v>
       </c>
@@ -10865,6 +11935,10 @@
       <c r="G273" t="s">
         <v>648</v>
       </c>
+      <c r="H273" s="8">
+        <f>VLOOKUP(G273,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I273" t="s">
         <v>53</v>
       </c>
@@ -10895,6 +11969,10 @@
       <c r="G274" t="s">
         <v>647</v>
       </c>
+      <c r="H274" s="8">
+        <f>VLOOKUP(G274,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I274" t="s">
         <v>23</v>
       </c>
@@ -10925,6 +12003,10 @@
       <c r="G275" t="s">
         <v>12</v>
       </c>
+      <c r="H275" s="8">
+        <f>VLOOKUP(G275,Fees!$A$2:$B$24,2,0)</f>
+        <v>27</v>
+      </c>
       <c r="I275" t="s">
         <v>53</v>
       </c>
@@ -10955,6 +12037,10 @@
       <c r="G276" t="s">
         <v>68</v>
       </c>
+      <c r="H276" s="8">
+        <f>VLOOKUP(G276,Fees!$A$2:$B$24,2,0)</f>
+        <v>49</v>
+      </c>
       <c r="I276" t="s">
         <v>13</v>
       </c>
@@ -10985,6 +12071,10 @@
       <c r="G277" t="s">
         <v>648</v>
       </c>
+      <c r="H277" s="8">
+        <f>VLOOKUP(G277,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I277" t="s">
         <v>53</v>
       </c>
@@ -11015,6 +12105,10 @@
       <c r="G278" t="s">
         <v>647</v>
       </c>
+      <c r="H278" s="8">
+        <f>VLOOKUP(G278,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I278" t="s">
         <v>13</v>
       </c>
@@ -11045,6 +12139,10 @@
       <c r="G279" t="s">
         <v>647</v>
       </c>
+      <c r="H279" s="8">
+        <f>VLOOKUP(G279,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I279" t="s">
         <v>23</v>
       </c>
@@ -11078,6 +12176,10 @@
       <c r="G280" t="s">
         <v>95</v>
       </c>
+      <c r="H280" s="8">
+        <f>VLOOKUP(G280,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I280" t="s">
         <v>23</v>
       </c>
@@ -11108,6 +12210,10 @@
       <c r="G281" t="s">
         <v>646</v>
       </c>
+      <c r="H281" s="8">
+        <f>VLOOKUP(G281,Fees!$A$2:$B$24,2,0)</f>
+        <v>60</v>
+      </c>
       <c r="I281" t="s">
         <v>23</v>
       </c>
@@ -11138,6 +12244,10 @@
       <c r="G282" t="s">
         <v>648</v>
       </c>
+      <c r="H282" s="8">
+        <f>VLOOKUP(G282,Fees!$A$2:$B$24,2,0)</f>
+        <v>35</v>
+      </c>
       <c r="I282" t="s">
         <v>23</v>
       </c>
@@ -11171,6 +12281,10 @@
       <c r="G283" t="s">
         <v>34</v>
       </c>
+      <c r="H283" s="8">
+        <f>VLOOKUP(G283,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I283" t="s">
         <v>53</v>
       </c>
@@ -11204,6 +12318,10 @@
       <c r="G284" t="s">
         <v>95</v>
       </c>
+      <c r="H284" s="8">
+        <f>VLOOKUP(G284,Fees!$A$2:$B$24,2,0)</f>
+        <v>24</v>
+      </c>
       <c r="I284" t="s">
         <v>53</v>
       </c>
@@ -11234,6 +12352,10 @@
       <c r="G285" t="s">
         <v>18</v>
       </c>
+      <c r="H285" s="8">
+        <f>VLOOKUP(G285,Fees!$A$2:$B$24,2,0)</f>
+        <v>36</v>
+      </c>
       <c r="I285" t="s">
         <v>23</v>
       </c>
@@ -11267,6 +12389,10 @@
       <c r="G286" t="s">
         <v>34</v>
       </c>
+      <c r="H286" s="8">
+        <f>VLOOKUP(G286,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I286" t="s">
         <v>13</v>
       </c>
@@ -11297,6 +12423,10 @@
       <c r="G287" t="s">
         <v>34</v>
       </c>
+      <c r="H287" s="8">
+        <f>VLOOKUP(G287,Fees!$A$2:$B$24,2,0)</f>
+        <v>74</v>
+      </c>
       <c r="I287" t="s">
         <v>53</v>
       </c>
@@ -11327,6 +12457,10 @@
       <c r="G288" t="s">
         <v>22</v>
       </c>
+      <c r="H288" s="8">
+        <f>VLOOKUP(G288,Fees!$A$2:$B$24,2,0)</f>
+        <v>86</v>
+      </c>
       <c r="I288" t="s">
         <v>53</v>
       </c>
@@ -11357,6 +12491,10 @@
       <c r="G289" t="s">
         <v>647</v>
       </c>
+      <c r="H289" s="8">
+        <f>VLOOKUP(G289,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I289" t="s">
         <v>53</v>
       </c>
@@ -11387,6 +12525,10 @@
       <c r="G290" t="s">
         <v>647</v>
       </c>
+      <c r="H290" s="8">
+        <f>VLOOKUP(G290,Fees!$A$2:$B$24,2,0)</f>
+        <v>58</v>
+      </c>
       <c r="I290" t="s">
         <v>13</v>
       </c>
@@ -11417,6 +12559,10 @@
       <c r="G291" t="s">
         <v>28</v>
       </c>
+      <c r="H291" s="8">
+        <f>VLOOKUP(G291,Fees!$A$2:$B$24,2,0)</f>
+        <v>46</v>
+      </c>
       <c r="I291" t="s">
         <v>35</v>
       </c>
@@ -11447,6 +12593,10 @@
       <c r="G292" t="s">
         <v>184</v>
       </c>
+      <c r="H292" s="8">
+        <f>VLOOKUP(G292,Fees!$A$2:$B$24,2,0)</f>
+        <v>20</v>
+      </c>
       <c r="I292" t="s">
         <v>13</v>
       </c>
@@ -11476,6 +12626,10 @@
       </c>
       <c r="G293" t="s">
         <v>645</v>
+      </c>
+      <c r="H293" s="8">
+        <f>VLOOKUP(G293,Fees!$A$2:$B$24,2,0)</f>
+        <v>21</v>
       </c>
       <c r="I293" t="s">
         <v>13</v>
@@ -11497,7 +12651,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F26FAC0-CF21-4C5C-9A16-AA07552E806D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11706,7 +12862,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11737,6 +12893,10 @@
       <c r="B2">
         <v>86</v>
       </c>
+      <c r="C2" t="str">
+        <f>IF(B2&lt;50,"F",IF(B2&lt;60,"D",IF(B2&lt;70,"C",IF(B2&lt;80,"B",IF(B2&gt;80,"A")))))</f>
+        <v>A</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
@@ -11745,6 +12905,10 @@
       <c r="B3">
         <v>97</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C39" si="0">IF(B3&lt;50,"F",IF(B3&lt;60,"D",IF(B3&lt;70,"C",IF(B3&lt;80,"B",IF(B3&gt;80,"A")))))</f>
+        <v>A</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>656</v>
       </c>
@@ -11762,6 +12926,10 @@
       <c r="B4">
         <v>90</v>
       </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
       <c r="E4" t="s">
         <v>655</v>
       </c>
@@ -11779,6 +12947,10 @@
       <c r="B5">
         <v>79</v>
       </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
       <c r="E5" t="s">
         <v>655</v>
       </c>
@@ -11796,6 +12968,10 @@
       <c r="B6">
         <v>97</v>
       </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
       <c r="E6" t="s">
         <v>655</v>
       </c>
@@ -11813,6 +12989,10 @@
       <c r="B7">
         <v>95</v>
       </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
       <c r="E7" t="s">
         <v>655</v>
       </c>
@@ -11832,6 +13012,10 @@
       <c r="B8">
         <v>90</v>
       </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
       <c r="E8" t="s">
         <v>658</v>
       </c>
@@ -11849,6 +13033,10 @@
       <c r="B9">
         <v>77</v>
       </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
@@ -11857,6 +13045,10 @@
       <c r="B10">
         <v>75</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
@@ -11865,6 +13057,10 @@
       <c r="B11">
         <v>100</v>
       </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
@@ -11873,6 +13069,10 @@
       <c r="B12">
         <v>81</v>
       </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
@@ -11881,6 +13081,10 @@
       <c r="B13">
         <v>99</v>
       </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
@@ -11889,6 +13093,10 @@
       <c r="B14">
         <v>86</v>
       </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
@@ -11897,6 +13105,10 @@
       <c r="B15">
         <v>84</v>
       </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
@@ -11905,189 +13117,285 @@
       <c r="B16">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>9142</v>
       </c>
       <c r="B17">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>9124</v>
       </c>
       <c r="B18">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>9120</v>
       </c>
       <c r="B19">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>9178</v>
       </c>
       <c r="B20">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>9211</v>
       </c>
       <c r="B21">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>9169</v>
       </c>
       <c r="B22">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>9158</v>
       </c>
       <c r="B23">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>9194</v>
       </c>
       <c r="B24">
         <v>94</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>9197</v>
       </c>
       <c r="B25">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>9137</v>
       </c>
       <c r="B26">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>9146</v>
       </c>
       <c r="B27">
         <v>78</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>9181</v>
       </c>
       <c r="B28">
         <v>56</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>9152</v>
       </c>
       <c r="B29">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>9133</v>
       </c>
       <c r="B30">
         <v>78</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>9154</v>
       </c>
       <c r="B31">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>9204</v>
       </c>
       <c r="B32">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>9201</v>
       </c>
       <c r="B33">
         <v>89</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>9115</v>
       </c>
       <c r="B34">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>9166</v>
       </c>
       <c r="B35">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>9206</v>
       </c>
       <c r="B36">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>9141</v>
       </c>
       <c r="B37">
         <v>82</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>9164</v>
       </c>
       <c r="B38">
         <v>99</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>9161</v>
       </c>
       <c r="B39">
         <v>90</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
       </c>
     </row>
   </sheetData>
@@ -12097,15 +13405,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016FB1796C7A54349A67930A9E98FFA33" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ba6c76ce8d155063fb686ff06cfeb3e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="39ef0995-f340-485f-a44a-0c60afb7c13e" xmlns:ns3="aa504cd8-0e2d-49cd-b0df-da45d3cad8b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="10b0dce4f4bc17346401271424b5492e" ns2:_="" ns3:_="">
     <xsd:import namespace="39ef0995-f340-485f-a44a-0c60afb7c13e"/>
@@ -12322,6 +13621,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -12329,14 +13637,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008C3664-79CC-47AF-BD02-421E7E2B0E15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B52961C-A0B1-4800-B00E-0B36B0F7D5F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12351,6 +13651,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{008C3664-79CC-47AF-BD02-421E7E2B0E15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>